<commit_message>
[NEW] Added new methods
</commit_message>
<xml_diff>
--- a/EfficientSorting/EfficientSorting_Template.xlsx
+++ b/EfficientSorting/EfficientSorting_Template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27421"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,20 +38,20 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
+    <t>Temps (ms)</t>
+  </si>
+  <si>
     <t>n</t>
   </si>
   <si>
     <t>Selection Sort</t>
-  </si>
-  <si>
-    <t>Temps (ms)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -112,10 +118,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -136,7 +142,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="ca-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -198,7 +204,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -410,7 +416,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -448,7 +454,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1842319647"/>
@@ -528,7 +534,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -566,7 +572,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1842317919"/>
@@ -608,7 +614,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -645,7 +651,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1256,7 +1262,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1558,31 +1564,31 @@
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.8125" customWidth="1"/>
+    <col min="1" max="1" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.5">
-      <c r="B1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+    <row r="1" spans="1:16">
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:16">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2">
         <v>10</v>
@@ -1618,9 +1624,9 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1650,8 +1656,8 @@
         <v>191791</v>
       </c>
     </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.5">
-      <c r="K17" s="5"/>
+    <row r="17" spans="11:11">
+      <c r="K17" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>